<commit_message>
post and put methods.  error messages when query or body is not matched.
</commit_message>
<xml_diff>
--- a/server/endpoints.xlsx
+++ b/server/endpoints.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orct\code\lydia.test.automation\server\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orct\code\simple-api-test-automation\server\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
   <si>
     <t>GET</t>
   </si>
@@ -53,9 +53,6 @@
     <t>/entitlements</t>
   </si>
   <si>
-    <t>params</t>
-  </si>
-  <si>
     <t>/wallets</t>
   </si>
   <si>
@@ -93,6 +90,36 @@
   </si>
   <si>
     <t>{ "message": "Hello World!" }</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>{
+  "name": "Pol",
+  "lastName": "Puig"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "id": "1"
+}</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>{
+  "id": "1",
+  "name": "Pol",
+  "lastName": "New Last Name"
+}</t>
+  </si>
+  <si>
+    <t>body</t>
+  </si>
+  <si>
+    <t>query</t>
   </si>
 </sst>
 </file>
@@ -475,21 +502,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -497,122 +525,161 @@
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="1" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="1" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="1" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="1" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adapted to api-server-sim library.
</commit_message>
<xml_diff>
--- a/server/endpoints.xlsx
+++ b/server/endpoints.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orct\code\simple-api-test-automation\server\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\api-server-sim\test_server\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01675978-47EF-47D9-9463-42A961FE38E3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="16395" windowHeight="10545"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="16395" windowHeight="10546" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="34">
   <si>
     <t>GET</t>
   </si>
@@ -95,37 +96,55 @@
     <t>POST</t>
   </si>
   <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>body</t>
+  </si>
+  <si>
+    <t>query</t>
+  </si>
+  <si>
+    <t>/users/1/books/2</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>/user/login</t>
+  </si>
+  <si>
     <t>{
-  "name": "Pol",
-  "lastName": "Puig"
+  "username": "user.maker",
+  "password": "1234"
 }</t>
   </si>
   <si>
+    <t>{ "errorMessage": "Not authorized user"}</t>
+  </si>
+  <si>
     <t>{
-  "id": "1"
+  "id": 1
 }</t>
   </si>
   <si>
-    <t>PUT</t>
-  </si>
-  <si>
     <t>{
-  "id": "1",
-  "name": "Pol",
+  "name": "John",
+  "lastName": "Smith"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "id": 1,
+  "name": "John",
   "lastName": "New Last Name"
 }</t>
-  </si>
-  <si>
-    <t>body</t>
-  </si>
-  <si>
-    <t>query</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -142,7 +161,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -152,6 +171,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
       </patternFill>
     </fill>
   </fills>
@@ -179,17 +203,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
+    <cellStyle name="Accent6" xfId="2" builtinId="49"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -501,23 +530,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="38.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.06640625" customWidth="1"/>
+    <col min="4" max="4" width="15.46484375" customWidth="1"/>
+    <col min="5" max="5" width="5.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -525,160 +555,255 @@
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="4">
+        <v>200</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="4">
+        <v>200</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="C4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="4">
+        <v>403</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="C5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="4">
+        <v>201</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="4">
+        <v>200</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="C7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="4">
+        <v>200</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="4">
+        <v>200</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="C9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="4">
+        <v>404</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1" t="s">
+      <c r="C10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E10" s="4">
+        <v>200</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="1" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1" t="s">
+      <c r="C11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E11" s="4">
+        <v>200</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="1" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="1" t="s">
+      <c r="C12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="4">
+        <v>200</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="1" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="1" t="s">
+      <c r="C13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="4">
+        <v>200</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>